<commit_message>
add: Acme Login test case
</commit_message>
<xml_diff>
--- a/Loan Quotes.xlsx
+++ b/Loan Quotes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ionut-mihai.nicula\Documents\UiPath\UiBank Loan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunil\Documents\UiPath\test suite\Create Loan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1EA52A-A5C3-4D5D-AC4D-B1ED7DBDDD35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D126C30C-0758-4A5D-9FB5-67ACCF7E699F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AB1519B2-5C0E-448B-8AC7-B3DEE8C41096}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AB1519B2-5C0E-448B-8AC7-B3DEE8C41096}"/>
   </bookViews>
   <sheets>
     <sheet name="Loan Quotes" sheetId="1" r:id="rId1"/>
@@ -452,22 +452,22 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="6" customWidth="1"/>
-    <col min="2" max="5" width="20.5703125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="52.85546875" style="1" customWidth="1"/>
-    <col min="9" max="10" width="12.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" style="6" customWidth="1"/>
+    <col min="2" max="5" width="20.5546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="52.88671875" style="1" customWidth="1"/>
+    <col min="9" max="10" width="12.5546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" style="2" customWidth="1"/>
     <col min="12" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -495,7 +495,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="7">
         <v>120000</v>
@@ -516,7 +516,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -542,7 +542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -568,7 +568,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -594,7 +594,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -620,7 +620,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -646,7 +646,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>

</xml_diff>